<commit_message>
fix: todo el sitio es reparado
</commit_message>
<xml_diff>
--- a/src/Head.xlsx
+++ b/src/Head.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12450"/>
+    <workbookView windowWidth="27945" windowHeight="12450" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="5" r:id="rId1"/>
     <sheet name="GIT" sheetId="7" r:id="rId2"/>
-    <sheet name="Vite" sheetId="6" r:id="rId3"/>
-    <sheet name="BootstrapTABLE" sheetId="2" r:id="rId4"/>
-    <sheet name="GittTABLE" sheetId="3" r:id="rId5"/>
-    <sheet name="script" sheetId="8" r:id="rId6"/>
+    <sheet name="BootstrapTABLE" sheetId="2" r:id="rId3"/>
+    <sheet name="GittTABLE" sheetId="3" r:id="rId4"/>
+    <sheet name="script" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="73">
   <si>
     <t>Título</t>
   </si>
@@ -220,22 +219,22 @@
     <t>&lt;/head&gt;</t>
   </si>
   <si>
-    <t>Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero.</t>
-  </si>
-  <si>
-    <t>https://eduardoherreraf.github.io/git@como_eliminar_el_ultimo_commit_de_git.html</t>
-  </si>
-  <si>
-    <t>Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero.</t>
+    <t>Instalación de Bootstrap V5, NPM y PARCEL - Ing. Eduardo Herrera Forero.</t>
   </si>
   <si>
     <t>https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html</t>
   </si>
   <si>
-    <t>Índice de Bootstrap - Ing. Eduardo Herrera Forero.</t>
-  </si>
-  <si>
-    <t>Este es el índice en donde se encontraran todos los artículos de la Librería CSS Bootstrap que se han publicado en este sitio web.</t>
+    <t>La guía oficial sobre cómo incluir y empaquetar el CSS y JavaScript de Bootstrap en un proyecto utilizando Parcel.</t>
+  </si>
+  <si>
+    <t>Índice de javascript - Ing. Eduardo Herrera Forero.</t>
+  </si>
+  <si>
+    <t>https://eduardoherreraf.github.io/javascript.html</t>
+  </si>
+  <si>
+    <t>Índice que enumera todos los artículos del lenguaje de programación Javascript publicados en este sitio web</t>
   </si>
   <si>
     <t>&lt;meta name="robots" content="noindex, follow" /&gt;</t>
@@ -894,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1240,8 +1239,788 @@
   <sheetPr/>
   <dimension ref="A1:XFD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="0.158333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2"/>
+    <col min="3" max="3" width="139.991666666667" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2"/>
+    <col min="5" max="5" width="35" style="2" customWidth="1"/>
+    <col min="6" max="16383" width="11" style="2"/>
+    <col min="16384" max="16384" width="11" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16384">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD1" s="2"/>
+    </row>
+    <row r="2" spans="2:16384">
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD2" s="2"/>
+    </row>
+    <row r="3" spans="2:16384">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD3" s="2"/>
+    </row>
+    <row r="4" ht="6" customHeight="1" spans="2:16384">
+      <c r="B4" s="8"/>
+      <c r="XFD4" s="2"/>
+    </row>
+    <row r="5" spans="1:16384">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="str">
+        <f t="shared" ref="B5:B8" si="0">A5</f>
+        <v>&lt;head&gt;</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD5" s="2"/>
+    </row>
+    <row r="6" spans="1:16384">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;!-- Metaetiquetas --&gt;</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD6" s="2"/>
+    </row>
+    <row r="7" spans="1:16384">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;meta charset="utf-8" /&gt;</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD7" s="2"/>
+    </row>
+    <row r="8" spans="1:16384">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;meta name="viewport" content="width=device-width, initial-scale=1" /&gt;</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD8" s="2"/>
+    </row>
+    <row r="9" spans="1:16384">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9" t="str">
+        <f>CONCATENATE(E9,$C$1,F9)</f>
+        <v>&lt;meta name="description" content="Ing. Eduardo Herrera Forero." /&gt;</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="XFD9" s="2"/>
+    </row>
+    <row r="10" spans="1:16384">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="9" t="str">
+        <f t="shared" ref="B10:B13" si="1">A10</f>
+        <v>&lt;meta name="author" content="Ing. Eduardo Herrera Forero" /&gt;</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD10" s="2"/>
+    </row>
+    <row r="11" spans="1:16384">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name="application-name" content="EHF" /&gt;</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD11" s="2"/>
+    </row>
+    <row r="12" spans="1:16384">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name="robots" content="index, follow" /&gt;</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD12" s="2"/>
+    </row>
+    <row r="13" spans="1:16384">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name="google" content="notranslate" /&gt;</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="XFD13" s="2"/>
+    </row>
+    <row r="14" spans="1:16384">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>CONCATENATE(E14,$C$2,$F$9)</f>
+        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/bootstrap.html" /&gt;</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="XFD14" s="2"/>
+    </row>
+    <row r="15" spans="1:16384">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="9" t="str">
+        <f t="shared" ref="B15:B18" si="2">A15</f>
+        <v>&lt;!-- Fin Metaetiquetas --&gt;</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD15" s="2"/>
+    </row>
+    <row r="16" spans="2:16384">
+      <c r="B16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD16" s="2"/>
+    </row>
+    <row r="17" spans="1:16384">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;!-- Open Graph data --&gt;</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD17" s="2"/>
+    </row>
+    <row r="18" spans="1:16384">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;meta property="og:type" content="website" /&gt;</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD18" s="2"/>
+    </row>
+    <row r="19" spans="1:16384">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9" t="str">
+        <f>CONCATENATE(E19,$C$1,F9)</f>
+        <v>&lt;meta property="og:title" content="Ing. Eduardo Herrera Forero." /&gt;</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="XFD19" s="2"/>
+    </row>
+    <row r="20" spans="1:16384">
+      <c r="A20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="9" t="str">
+        <f>CONCATENATE(E20,$C$3,$F$9)</f>
+        <v>&lt;meta property="og:description" content="Esta es la Página Web del ingeniero Eduardo Herrera Forero y sus publicaciones." /&gt;</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="XFD20" s="2"/>
+    </row>
+    <row r="21" spans="1:16384">
+      <c r="A21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="9" t="str">
+        <f t="shared" ref="B21:B25" si="3">A21</f>
+        <v>&lt;meta property="og:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD21" s="2"/>
+    </row>
+    <row r="22" spans="1:16384">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;meta property="og:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"/&gt;</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD22" s="2"/>
+    </row>
+    <row r="23" spans="1:16384">
+      <c r="A23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="9" t="str">
+        <f>CONCATENATE(E23,$C$2,$F$9)</f>
+        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/bootstrap.html" /&gt;</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="XFD23" s="2"/>
+    </row>
+    <row r="24" spans="1:16384">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;meta property="og:locale" content="es_CO" /&gt;</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD24" s="2"/>
+    </row>
+    <row r="25" spans="1:16384">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;!-- fin Open Graph data --&gt;</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD25" s="2"/>
+    </row>
+    <row r="26" spans="2:16384">
+      <c r="B26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD26" s="2"/>
+    </row>
+    <row r="27" spans="1:16384">
+      <c r="A27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="9" t="str">
+        <f t="shared" ref="B27:B29" si="4">A27</f>
+        <v>&lt;!-- Twitter cards --&gt;</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD27" s="2"/>
+    </row>
+    <row r="28" spans="1:16384">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;meta name="twitter:card" content="summary" /&gt;</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD28" s="2"/>
+    </row>
+    <row r="29" spans="1:16384">
+      <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;meta name="twitter:site" content="@ehfeduardo" /&gt;</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD29" s="2"/>
+    </row>
+    <row r="30" spans="1:16384">
+      <c r="A30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="9" t="str">
+        <f>CONCATENATE(E30,$C$1,$F$9)</f>
+        <v>&lt;meta name="twitter:title" content="Ing. Eduardo Herrera Forero." /&gt;</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="XFD30" s="2"/>
+    </row>
+    <row r="31" spans="1:16384">
+      <c r="A31" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="9" t="str">
+        <f>CONCATENATE(E31,$C$3,$F$9)</f>
+        <v>&lt;meta name="twitter:description" content="Esta es la Página Web del ingeniero Eduardo Herrera Forero y sus publicaciones." /&gt;</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="XFD31" s="2"/>
+    </row>
+    <row r="32" spans="1:16384">
+      <c r="A32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="9" t="str">
+        <f t="shared" ref="B32:B34" si="5">A32</f>
+        <v>&lt;meta name="twitter:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD32" s="2"/>
+    </row>
+    <row r="33" spans="1:16384">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;meta name="twitter:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"&gt;</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD33" s="2"/>
+    </row>
+    <row r="34" spans="1:16384">
+      <c r="A34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;!-- Fin Twitter cards --&gt;</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD34" s="2"/>
+    </row>
+    <row r="35" spans="2:16384">
+      <c r="B35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD35" s="2"/>
+    </row>
+    <row r="36" spans="1:16384">
+      <c r="A36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="9" t="str">
+        <f t="shared" ref="B36:B45" si="6">A36</f>
+        <v>&lt;!-- iconos --&gt;</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD36" s="2"/>
+    </row>
+    <row r="37" spans="1:16384">
+      <c r="A37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;link rel="apple-touch-icon" sizes="180x180" href="apple-touch-icon.png" /&gt;</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD37" s="2"/>
+    </row>
+    <row r="38" spans="1:16384">
+      <c r="A38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;link rel="icon" type="image/png" sizes="32x32" href="favicon-32x32.png" /&gt;</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD38" s="2"/>
+    </row>
+    <row r="39" spans="1:16384">
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;link rel="icon" type="image/png" sizes="192x192" href="android-chrome-192x192.png"/&gt;</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD39" s="2"/>
+    </row>
+    <row r="40" spans="1:16384">
+      <c r="A40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;link rel="icon" type="image/png" sizes="16x16" href="favicon-16x16.png" /&gt;</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD40" s="2"/>
+    </row>
+    <row r="41" spans="1:16384">
+      <c r="A41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;link rel="manifest" href="site.webmanifest" /&gt;</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD41" s="2"/>
+    </row>
+    <row r="42" spans="1:16384">
+      <c r="A42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;link rel="mask-icon" href="safari-pinned-tab.svg" color="#5bbad5" /&gt;</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD42" s="2"/>
+    </row>
+    <row r="43" spans="1:16384">
+      <c r="A43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;meta name="msapplication-TileColor" content="#da532c" /&gt;</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD43" s="2"/>
+    </row>
+    <row r="44" spans="1:16384">
+      <c r="A44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;meta name="theme-color" content="#ffffff" /&gt;</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD44" s="2"/>
+    </row>
+    <row r="45" spans="1:16384">
+      <c r="A45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;!-- fin iconos --&gt;</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD45" s="2"/>
+    </row>
+    <row r="46" spans="2:16384">
+      <c r="B46" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD46" s="2"/>
+    </row>
+    <row r="47" spans="1:16384">
+      <c r="A47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="9" t="str">
+        <f t="shared" ref="B47:B51" si="7">A47</f>
+        <v>&lt;title&gt;</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD47" s="2"/>
+    </row>
+    <row r="48" spans="1:16384">
+      <c r="A48" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="9" t="str">
+        <f>C1</f>
+        <v>Ing. Eduardo Herrera Forero.</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD48" s="2"/>
+    </row>
+    <row r="49" spans="1:16384">
+      <c r="A49" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;/title&gt;</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD49" s="2"/>
+    </row>
+    <row r="50" spans="2:16384">
+      <c r="B50" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD50" s="2"/>
+    </row>
+    <row r="51" spans="1:16384">
+      <c r="A51" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;script type="module" defer src="./js/main.js"&gt;&lt;/script&gt;</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD51" s="2"/>
+    </row>
+    <row r="52" spans="2:16384">
+      <c r="B52" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD52" s="2"/>
+    </row>
+    <row r="53" spans="1:16384">
+      <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="9" t="str">
+        <f>A53</f>
+        <v>&lt;meta name="google-site-verification" content="2H5ZMCD1_xl7oxaiqnopfdQBnIXVIOfmW0UBSa5sQJc"/&gt;</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD53" s="2"/>
+    </row>
+    <row r="54" spans="1:16384">
+      <c r="A54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="9" t="str">
+        <f>A54</f>
+        <v>&lt;/head&gt;</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="XFD54" s="2"/>
+    </row>
+    <row r="55" spans="16384:16384">
+      <c r="XFD55" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/bootstrap.html"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:XFD55"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1264,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1276,7 +2055,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -1288,7 +2067,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -1360,8 +2139,8 @@
         <v>11</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f>CONCATENATE(E9,$C$1,F9)</f>
-        <v>&lt;meta name="description" content="Ing. Eduardo Herrera Forero." /&gt;</v>
+        <f>CONCATENATE(E9,$C$3,F9)</f>
+        <v>&lt;meta name="description" content="La guía oficial sobre cómo incluir y empaquetar el CSS y JavaScript de Bootstrap en un proyecto utilizando Parcel." /&gt;</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
@@ -1440,7 +2219,7 @@
       </c>
       <c r="B14" s="9" t="str">
         <f>CONCATENATE(E14,$C$2,$F$9)</f>
-        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/bootstrap.html" /&gt;</v>
+        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html" /&gt;</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
@@ -1509,7 +2288,7 @@
       </c>
       <c r="B19" s="9" t="str">
         <f>CONCATENATE(E19,$C$1,F9)</f>
-        <v>&lt;meta property="og:title" content="Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta property="og:title" content="Instalación de Bootstrap V5, NPM y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
@@ -1526,7 +2305,7 @@
       </c>
       <c r="B20" s="9" t="str">
         <f>CONCATENATE(E20,$C$3,$F$9)</f>
-        <v>&lt;meta property="og:description" content="Esta es la Página Web del ingeniero Eduardo Herrera Forero y sus publicaciones." /&gt;</v>
+        <v>&lt;meta property="og:description" content="La guía oficial sobre cómo incluir y empaquetar el CSS y JavaScript de Bootstrap en un proyecto utilizando Parcel." /&gt;</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
@@ -1571,7 +2350,7 @@
       </c>
       <c r="B23" s="9" t="str">
         <f>CONCATENATE(E23,$C$2,$F$9)</f>
-        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/bootstrap.html" /&gt;</v>
+        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html" /&gt;</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9" t="s">
@@ -1668,7 +2447,7 @@
       </c>
       <c r="B30" s="9" t="str">
         <f>CONCATENATE(E30,$C$1,$F$9)</f>
-        <v>&lt;meta name="twitter:title" content="Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta name="twitter:title" content="Instalación de Bootstrap V5, NPM y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
@@ -1685,7 +2464,7 @@
       </c>
       <c r="B31" s="9" t="str">
         <f>CONCATENATE(E31,$C$3,$F$9)</f>
-        <v>&lt;meta name="twitter:description" content="Esta es la Página Web del ingeniero Eduardo Herrera Forero y sus publicaciones." /&gt;</v>
+        <v>&lt;meta name="twitter:description" content="La guía oficial sobre cómo incluir y empaquetar el CSS y JavaScript de Bootstrap en un proyecto utilizando Parcel." /&gt;</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
@@ -1918,7 +2697,7 @@
       </c>
       <c r="B48" s="9" t="str">
         <f>C1</f>
-        <v>Ing. Eduardo Herrera Forero.</v>
+        <v>Instalación de Bootstrap V5, NPM y PARCEL - Ing. Eduardo Herrera Forero.</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9" t="s">
@@ -2007,787 +2786,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/bootstrap.html"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:XFD55"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="0.158333333333333" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="139.991666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2"/>
-    <col min="5" max="5" width="35" style="2" customWidth="1"/>
-    <col min="6" max="16383" width="11" style="2"/>
-    <col min="16384" max="16384" width="11" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:16384">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD1" s="2"/>
-    </row>
-    <row r="2" spans="2:16384">
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD2" s="2"/>
-    </row>
-    <row r="3" spans="2:16384">
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD3" s="2"/>
-    </row>
-    <row r="4" ht="6" customHeight="1" spans="2:16384">
-      <c r="B4" s="8"/>
-      <c r="XFD4" s="2"/>
-    </row>
-    <row r="5" spans="1:16384">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9" t="str">
-        <f t="shared" ref="B5:B8" si="0">A5</f>
-        <v>&lt;head&gt;</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD5" s="2"/>
-    </row>
-    <row r="6" spans="1:16384">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;!-- Metaetiquetas --&gt;</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD6" s="2"/>
-    </row>
-    <row r="7" spans="1:16384">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;meta charset="utf-8" /&gt;</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD7" s="2"/>
-    </row>
-    <row r="8" spans="1:16384">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;meta name="viewport" content="width=device-width, initial-scale=1" /&gt;</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD8" s="2"/>
-    </row>
-    <row r="9" spans="1:16384">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="9" t="str">
-        <f>CONCATENATE(E9,$C$1,F9)</f>
-        <v>&lt;meta name="description" content="Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="XFD9" s="2"/>
-    </row>
-    <row r="10" spans="1:16384">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f t="shared" ref="B10:B13" si="1">A10</f>
-        <v>&lt;meta name="author" content="Ing. Eduardo Herrera Forero" /&gt;</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD10" s="2"/>
-    </row>
-    <row r="11" spans="1:16384">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta name="application-name" content="EHF" /&gt;</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD11" s="2"/>
-    </row>
-    <row r="12" spans="1:16384">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta name="robots" content="index, follow" /&gt;</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD12" s="2"/>
-    </row>
-    <row r="13" spans="1:16384">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta name="google" content="notranslate" /&gt;</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="XFD13" s="2"/>
-    </row>
-    <row r="14" spans="1:16384">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="9" t="str">
-        <f>CONCATENATE(E14,$C$2,$F$9)</f>
-        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/git@como_eliminar_el_ultimo_commit_de_git.html" /&gt;</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="XFD14" s="2"/>
-    </row>
-    <row r="15" spans="1:16384">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="9" t="str">
-        <f t="shared" ref="B15:B18" si="2">A15</f>
-        <v>&lt;!-- Fin Metaetiquetas --&gt;</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD15" s="2"/>
-    </row>
-    <row r="16" spans="2:16384">
-      <c r="B16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD16" s="2"/>
-    </row>
-    <row r="17" spans="1:16384">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;!-- Open Graph data --&gt;</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD17" s="2"/>
-    </row>
-    <row r="18" spans="1:16384">
-      <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;meta property="og:type" content="website" /&gt;</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD18" s="2"/>
-    </row>
-    <row r="19" spans="1:16384">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="9" t="str">
-        <f>CONCATENATE(E19,$C$1,F9)</f>
-        <v>&lt;meta property="og:title" content="Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="XFD19" s="2"/>
-    </row>
-    <row r="20" spans="1:16384">
-      <c r="A20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="9" t="str">
-        <f>CONCATENATE(E20,$C$3,$F$9)</f>
-        <v>&lt;meta property="og:description" content="Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="XFD20" s="2"/>
-    </row>
-    <row r="21" spans="1:16384">
-      <c r="A21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="9" t="str">
-        <f t="shared" ref="B21:B25" si="3">A21</f>
-        <v>&lt;meta property="og:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD21" s="2"/>
-    </row>
-    <row r="22" spans="1:16384">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;meta property="og:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"/&gt;</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD22" s="2"/>
-    </row>
-    <row r="23" spans="1:16384">
-      <c r="A23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="9" t="str">
-        <f>CONCATENATE(E23,$C$2,$F$9)</f>
-        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/git@como_eliminar_el_ultimo_commit_de_git.html" /&gt;</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="XFD23" s="2"/>
-    </row>
-    <row r="24" spans="1:16384">
-      <c r="A24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;meta property="og:locale" content="es_CO" /&gt;</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD24" s="2"/>
-    </row>
-    <row r="25" spans="1:16384">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;!-- fin Open Graph data --&gt;</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD25" s="2"/>
-    </row>
-    <row r="26" spans="2:16384">
-      <c r="B26" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD26" s="2"/>
-    </row>
-    <row r="27" spans="1:16384">
-      <c r="A27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="9" t="str">
-        <f t="shared" ref="B27:B29" si="4">A27</f>
-        <v>&lt;!-- Twitter cards --&gt;</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD27" s="2"/>
-    </row>
-    <row r="28" spans="1:16384">
-      <c r="A28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;meta name="twitter:card" content="summary" /&gt;</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD28" s="2"/>
-    </row>
-    <row r="29" spans="1:16384">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;meta name="twitter:site" content="@ehfeduardo" /&gt;</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD29" s="2"/>
-    </row>
-    <row r="30" spans="1:16384">
-      <c r="A30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="9" t="str">
-        <f>CONCATENATE(E30,$C$1,$F$9)</f>
-        <v>&lt;meta name="twitter:title" content="Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="XFD30" s="2"/>
-    </row>
-    <row r="31" spans="1:16384">
-      <c r="A31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="9" t="str">
-        <f>CONCATENATE(E31,$C$3,$F$9)</f>
-        <v>&lt;meta name="twitter:description" content="Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="XFD31" s="2"/>
-    </row>
-    <row r="32" spans="1:16384">
-      <c r="A32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="9" t="str">
-        <f t="shared" ref="B32:B34" si="5">A32</f>
-        <v>&lt;meta name="twitter:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD32" s="2"/>
-    </row>
-    <row r="33" spans="1:16384">
-      <c r="A33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;meta name="twitter:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"&gt;</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD33" s="2"/>
-    </row>
-    <row r="34" spans="1:16384">
-      <c r="A34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;!-- Fin Twitter cards --&gt;</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD34" s="2"/>
-    </row>
-    <row r="35" spans="2:16384">
-      <c r="B35" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD35" s="2"/>
-    </row>
-    <row r="36" spans="1:16384">
-      <c r="A36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="9" t="str">
-        <f t="shared" ref="B36:B45" si="6">A36</f>
-        <v>&lt;!-- iconos --&gt;</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD36" s="2"/>
-    </row>
-    <row r="37" spans="1:16384">
-      <c r="A37" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;link rel="apple-touch-icon" sizes="180x180" href="apple-touch-icon.png" /&gt;</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD37" s="2"/>
-    </row>
-    <row r="38" spans="1:16384">
-      <c r="A38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;link rel="icon" type="image/png" sizes="32x32" href="favicon-32x32.png" /&gt;</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD38" s="2"/>
-    </row>
-    <row r="39" spans="1:16384">
-      <c r="A39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;link rel="icon" type="image/png" sizes="192x192" href="android-chrome-192x192.png"/&gt;</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD39" s="2"/>
-    </row>
-    <row r="40" spans="1:16384">
-      <c r="A40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;link rel="icon" type="image/png" sizes="16x16" href="favicon-16x16.png" /&gt;</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD40" s="2"/>
-    </row>
-    <row r="41" spans="1:16384">
-      <c r="A41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;link rel="manifest" href="site.webmanifest" /&gt;</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD41" s="2"/>
-    </row>
-    <row r="42" spans="1:16384">
-      <c r="A42" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;link rel="mask-icon" href="safari-pinned-tab.svg" color="#5bbad5" /&gt;</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD42" s="2"/>
-    </row>
-    <row r="43" spans="1:16384">
-      <c r="A43" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;meta name="msapplication-TileColor" content="#da532c" /&gt;</v>
-      </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD43" s="2"/>
-    </row>
-    <row r="44" spans="1:16384">
-      <c r="A44" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;meta name="theme-color" content="#ffffff" /&gt;</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD44" s="2"/>
-    </row>
-    <row r="45" spans="1:16384">
-      <c r="A45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;!-- fin iconos --&gt;</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD45" s="2"/>
-    </row>
-    <row r="46" spans="2:16384">
-      <c r="B46" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD46" s="2"/>
-    </row>
-    <row r="47" spans="1:16384">
-      <c r="A47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" s="9" t="str">
-        <f t="shared" ref="B47:B51" si="7">A47</f>
-        <v>&lt;title&gt;</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD47" s="2"/>
-    </row>
-    <row r="48" spans="1:16384">
-      <c r="A48" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="9" t="str">
-        <f>C1</f>
-        <v>Como Eliminar el Último Commit de GIT - Ing. Eduardo Herrera Forero.</v>
-      </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD48" s="2"/>
-    </row>
-    <row r="49" spans="1:16384">
-      <c r="A49" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v>&lt;/title&gt;</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD49" s="2"/>
-    </row>
-    <row r="50" spans="2:16384">
-      <c r="B50" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD50" s="2"/>
-    </row>
-    <row r="51" spans="1:16384">
-      <c r="A51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v>&lt;script type="module" defer src="./js/main.js"&gt;&lt;/script&gt;</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD51" s="2"/>
-    </row>
-    <row r="52" spans="2:16384">
-      <c r="B52" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD52" s="2"/>
-    </row>
-    <row r="53" spans="1:16384">
-      <c r="A53" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="9" t="str">
-        <f>A53</f>
-        <v>&lt;meta name="google-site-verification" content="2H5ZMCD1_xl7oxaiqnopfdQBnIXVIOfmW0UBSa5sQJc"/&gt;</v>
-      </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD53" s="2"/>
-    </row>
-    <row r="54" spans="1:16384">
-      <c r="A54" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="9" t="str">
-        <f>A54</f>
-        <v>&lt;/head&gt;</v>
-      </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD54" s="2"/>
-    </row>
-    <row r="55" spans="16384:16384">
-      <c r="XFD55" s="2"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/git@como_eliminar_el_ultimo_commit_de_git.html" tooltip="https://eduardoherreraf.github.io/git@como_eliminar_el_ultimo_commit_de_git.html"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html" tooltip="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2797,7 +2796,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor theme="9" tint="0.8"/>
+  </sheetPr>
   <dimension ref="A1:XFD55"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -2823,8 +2824,8 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>64</v>
+      <c r="C1" t="s">
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2836,7 +2837,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -2847,8 +2848,8 @@
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>64</v>
+      <c r="C3" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -2920,8 +2921,8 @@
         <v>11</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f>CONCATENATE(E9,$C$1,F9)</f>
-        <v>&lt;meta name="description" content="Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <f>CONCATENATE(E9,$C$3,F9)</f>
+        <v>&lt;meta name="description" content="Índice que enumera todos los artículos del lenguaje de programación Javascript publicados en este sitio web" /&gt;</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
@@ -2940,7 +2941,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="9" t="str">
-        <f t="shared" ref="B10:B13" si="1">A10</f>
+        <f>A10</f>
         <v>&lt;meta name="author" content="Ing. Eduardo Herrera Forero" /&gt;</v>
       </c>
       <c r="C10" s="9"/>
@@ -2954,7 +2955,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>A11</f>
         <v>&lt;meta name="application-name" content="EHF" /&gt;</v>
       </c>
       <c r="C11" s="9"/>
@@ -2965,11 +2966,11 @@
     </row>
     <row r="12" spans="1:16384">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B12" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta name="robots" content="index, follow" /&gt;</v>
+        <f>A12</f>
+        <v>&lt;meta name="robots" content="noindex, follow" /&gt;</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9" t="s">
@@ -2982,15 +2983,12 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>A13</f>
         <v>&lt;meta name="google" content="notranslate" /&gt;</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
         <v>2</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="XFD13" s="2"/>
     </row>
@@ -3000,7 +2998,7 @@
       </c>
       <c r="B14" s="9" t="str">
         <f>CONCATENATE(E14,$C$2,$F$9)</f>
-        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html" /&gt;</v>
+        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/javascript.html" /&gt;</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
@@ -3016,7 +3014,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f t="shared" ref="B15:B18" si="2">A15</f>
+        <f t="shared" ref="B15:B18" si="1">A15</f>
         <v>&lt;!-- Fin Metaetiquetas --&gt;</v>
       </c>
       <c r="C15" s="9"/>
@@ -3040,7 +3038,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&lt;!-- Open Graph data --&gt;</v>
       </c>
       <c r="C17" s="9"/>
@@ -3054,7 +3052,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&lt;meta property="og:type" content="website" /&gt;</v>
       </c>
       <c r="C18" s="9"/>
@@ -3069,7 +3067,7 @@
       </c>
       <c r="B19" s="9" t="str">
         <f>CONCATENATE(E19,$C$1,F9)</f>
-        <v>&lt;meta property="og:title" content="Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta property="og:title" content="Índice de javascript - Ing. Eduardo Herrera Forero." /&gt;</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
@@ -3086,7 +3084,7 @@
       </c>
       <c r="B20" s="9" t="str">
         <f>CONCATENATE(E20,$C$3,$F$9)</f>
-        <v>&lt;meta property="og:description" content="Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta property="og:description" content="Índice que enumera todos los artículos del lenguaje de programación Javascript publicados en este sitio web" /&gt;</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
@@ -3102,7 +3100,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="9" t="str">
-        <f t="shared" ref="B21:B25" si="3">A21</f>
+        <f t="shared" ref="B21:B25" si="2">A21</f>
         <v>&lt;meta property="og:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
       </c>
       <c r="C21" s="9"/>
@@ -3116,7 +3114,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>&lt;meta property="og:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"/&gt;</v>
       </c>
       <c r="C22" s="9"/>
@@ -3131,7 +3129,7 @@
       </c>
       <c r="B23" s="9" t="str">
         <f>CONCATENATE(E23,$C$2,$F$9)</f>
-        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html" /&gt;</v>
+        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/javascript.html" /&gt;</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9" t="s">
@@ -3147,7 +3145,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>&lt;meta property="og:locale" content="es_CO" /&gt;</v>
       </c>
       <c r="C24" s="9"/>
@@ -3161,7 +3159,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>&lt;!-- fin Open Graph data --&gt;</v>
       </c>
       <c r="C25" s="9"/>
@@ -3185,7 +3183,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="9" t="str">
-        <f t="shared" ref="B27:B29" si="4">A27</f>
+        <f t="shared" ref="B27:B29" si="3">A27</f>
         <v>&lt;!-- Twitter cards --&gt;</v>
       </c>
       <c r="C27" s="9"/>
@@ -3199,7 +3197,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>&lt;meta name="twitter:card" content="summary" /&gt;</v>
       </c>
       <c r="C28" s="9"/>
@@ -3213,7 +3211,7 @@
         <v>38</v>
       </c>
       <c r="B29" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>&lt;meta name="twitter:site" content="@ehfeduardo" /&gt;</v>
       </c>
       <c r="C29" s="9"/>
@@ -3228,7 +3226,7 @@
       </c>
       <c r="B30" s="9" t="str">
         <f>CONCATENATE(E30,$C$1,$F$9)</f>
-        <v>&lt;meta name="twitter:title" content="Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta name="twitter:title" content="Índice de javascript - Ing. Eduardo Herrera Forero." /&gt;</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
@@ -3245,7 +3243,7 @@
       </c>
       <c r="B31" s="9" t="str">
         <f>CONCATENATE(E31,$C$3,$F$9)</f>
-        <v>&lt;meta name="twitter:description" content="Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta name="twitter:description" content="Índice que enumera todos los artículos del lenguaje de programación Javascript publicados en este sitio web" /&gt;</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
@@ -3261,7 +3259,7 @@
         <v>43</v>
       </c>
       <c r="B32" s="9" t="str">
-        <f t="shared" ref="B32:B34" si="5">A32</f>
+        <f t="shared" ref="B32:B34" si="4">A32</f>
         <v>&lt;meta name="twitter:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
       </c>
       <c r="C32" s="9"/>
@@ -3275,7 +3273,7 @@
         <v>44</v>
       </c>
       <c r="B33" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>&lt;meta name="twitter:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"&gt;</v>
       </c>
       <c r="C33" s="9"/>
@@ -3289,7 +3287,7 @@
         <v>45</v>
       </c>
       <c r="B34" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>&lt;!-- Fin Twitter cards --&gt;</v>
       </c>
       <c r="C34" s="9"/>
@@ -3313,7 +3311,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="9" t="str">
-        <f t="shared" ref="B36:B45" si="6">A36</f>
+        <f t="shared" ref="B36:B45" si="5">A36</f>
         <v>&lt;!-- iconos --&gt;</v>
       </c>
       <c r="C36" s="9"/>
@@ -3327,7 +3325,7 @@
         <v>47</v>
       </c>
       <c r="B37" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;link rel="apple-touch-icon" sizes="180x180" href="apple-touch-icon.png" /&gt;</v>
       </c>
       <c r="C37" s="9"/>
@@ -3341,7 +3339,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;link rel="icon" type="image/png" sizes="32x32" href="favicon-32x32.png" /&gt;</v>
       </c>
       <c r="C38" s="9"/>
@@ -3355,7 +3353,7 @@
         <v>49</v>
       </c>
       <c r="B39" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;link rel="icon" type="image/png" sizes="192x192" href="android-chrome-192x192.png"/&gt;</v>
       </c>
       <c r="C39" s="9"/>
@@ -3369,7 +3367,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;link rel="icon" type="image/png" sizes="16x16" href="favicon-16x16.png" /&gt;</v>
       </c>
       <c r="C40" s="9"/>
@@ -3383,7 +3381,7 @@
         <v>51</v>
       </c>
       <c r="B41" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;link rel="manifest" href="site.webmanifest" /&gt;</v>
       </c>
       <c r="C41" s="9"/>
@@ -3397,7 +3395,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;link rel="mask-icon" href="safari-pinned-tab.svg" color="#5bbad5" /&gt;</v>
       </c>
       <c r="C42" s="9"/>
@@ -3411,7 +3409,7 @@
         <v>53</v>
       </c>
       <c r="B43" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;meta name="msapplication-TileColor" content="#da532c" /&gt;</v>
       </c>
       <c r="C43" s="9"/>
@@ -3425,7 +3423,7 @@
         <v>54</v>
       </c>
       <c r="B44" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;meta name="theme-color" content="#ffffff" /&gt;</v>
       </c>
       <c r="C44" s="9"/>
@@ -3439,7 +3437,7 @@
         <v>55</v>
       </c>
       <c r="B45" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;!-- fin iconos --&gt;</v>
       </c>
       <c r="C45" s="9"/>
@@ -3463,7 +3461,7 @@
         <v>56</v>
       </c>
       <c r="B47" s="9" t="str">
-        <f t="shared" ref="B47:B51" si="7">A47</f>
+        <f t="shared" ref="B47:B51" si="6">A47</f>
         <v>&lt;title&gt;</v>
       </c>
       <c r="C47" s="9"/>
@@ -3478,7 +3476,7 @@
       </c>
       <c r="B48" s="9" t="str">
         <f>C1</f>
-        <v>Instalación de Bootstrap V5 con VITE y PARCEL - Ing. Eduardo Herrera Forero.</v>
+        <v>Índice de javascript - Ing. Eduardo Herrera Forero.</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9" t="s">
@@ -3491,7 +3489,7 @@
         <v>58</v>
       </c>
       <c r="B49" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>&lt;/title&gt;</v>
       </c>
       <c r="C49" s="9"/>
@@ -3515,7 +3513,7 @@
         <v>59</v>
       </c>
       <c r="B51" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>&lt;script type="module" defer src="./js/main.js"&gt;&lt;/script&gt;</v>
       </c>
       <c r="C51" s="9"/>
@@ -3567,7 +3565,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html" tooltip="https://eduardoherreraf.github.io/bootstrap@instalacion_de_bootstrap_v5_con_npm_y_parcel.html"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/javascript.html" tooltip="https://eduardoherreraf.github.io/javascript.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3580,7 +3578,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.8"/>
   </sheetPr>
-  <dimension ref="A1:XFD55"/>
+  <dimension ref="A1:XFD54"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -3606,785 +3604,6 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD1" s="2"/>
-    </row>
-    <row r="2" spans="2:16384">
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD2" s="2"/>
-    </row>
-    <row r="3" spans="2:16384">
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD3" s="2"/>
-    </row>
-    <row r="4" ht="6" customHeight="1" spans="2:16384">
-      <c r="B4" s="8"/>
-      <c r="XFD4" s="2"/>
-    </row>
-    <row r="5" spans="1:16384">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9" t="str">
-        <f t="shared" ref="B5:B8" si="0">A5</f>
-        <v>&lt;head&gt;</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD5" s="2"/>
-    </row>
-    <row r="6" spans="1:16384">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;!-- Metaetiquetas --&gt;</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD6" s="2"/>
-    </row>
-    <row r="7" spans="1:16384">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;meta charset="utf-8" /&gt;</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD7" s="2"/>
-    </row>
-    <row r="8" spans="1:16384">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;meta name="viewport" content="width=device-width, initial-scale=1" /&gt;</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD8" s="2"/>
-    </row>
-    <row r="9" spans="1:16384">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="9" t="str">
-        <f>CONCATENATE(E9,$C$1,F9)</f>
-        <v>&lt;meta name="description" content="Índice de Bootstrap - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="XFD9" s="2"/>
-    </row>
-    <row r="10" spans="1:16384">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f>A10</f>
-        <v>&lt;meta name="author" content="Ing. Eduardo Herrera Forero" /&gt;</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD10" s="2"/>
-    </row>
-    <row r="11" spans="1:16384">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="9" t="str">
-        <f>A11</f>
-        <v>&lt;meta name="application-name" content="EHF" /&gt;</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD11" s="2"/>
-    </row>
-    <row r="12" spans="1:16384">
-      <c r="A12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="9" t="str">
-        <f>A12</f>
-        <v>&lt;meta name="robots" content="noindex, follow" /&gt;</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD12" s="2"/>
-    </row>
-    <row r="13" spans="1:16384">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="9" t="str">
-        <f>A13</f>
-        <v>&lt;meta name="google" content="notranslate" /&gt;</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD13" s="2"/>
-    </row>
-    <row r="14" spans="1:16384">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="9" t="str">
-        <f>CONCATENATE(E14,$C$2,$F$9)</f>
-        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/bootstrap.html" /&gt;</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="XFD14" s="2"/>
-    </row>
-    <row r="15" spans="1:16384">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="9" t="str">
-        <f t="shared" ref="B15:B18" si="1">A15</f>
-        <v>&lt;!-- Fin Metaetiquetas --&gt;</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD15" s="2"/>
-    </row>
-    <row r="16" spans="2:16384">
-      <c r="B16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD16" s="2"/>
-    </row>
-    <row r="17" spans="1:16384">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;!-- Open Graph data --&gt;</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD17" s="2"/>
-    </row>
-    <row r="18" spans="1:16384">
-      <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta property="og:type" content="website" /&gt;</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD18" s="2"/>
-    </row>
-    <row r="19" spans="1:16384">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="9" t="str">
-        <f>CONCATENATE(E19,$C$1,F9)</f>
-        <v>&lt;meta property="og:title" content="Índice de Bootstrap - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="XFD19" s="2"/>
-    </row>
-    <row r="20" spans="1:16384">
-      <c r="A20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="9" t="str">
-        <f>CONCATENATE(E20,$C$3,$F$9)</f>
-        <v>&lt;meta property="og:description" content="Este es el índice en donde se encontraran todos los artículos de la Librería CSS Bootstrap que se han publicado en este sitio web." /&gt;</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="XFD20" s="2"/>
-    </row>
-    <row r="21" spans="1:16384">
-      <c r="A21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="9" t="str">
-        <f t="shared" ref="B21:B25" si="2">A21</f>
-        <v>&lt;meta property="og:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD21" s="2"/>
-    </row>
-    <row r="22" spans="1:16384">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;meta property="og:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"/&gt;</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD22" s="2"/>
-    </row>
-    <row r="23" spans="1:16384">
-      <c r="A23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="9" t="str">
-        <f>CONCATENATE(E23,$C$2,$F$9)</f>
-        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/bootstrap.html" /&gt;</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="XFD23" s="2"/>
-    </row>
-    <row r="24" spans="1:16384">
-      <c r="A24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;meta property="og:locale" content="es_CO" /&gt;</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD24" s="2"/>
-    </row>
-    <row r="25" spans="1:16384">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;!-- fin Open Graph data --&gt;</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD25" s="2"/>
-    </row>
-    <row r="26" spans="2:16384">
-      <c r="B26" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD26" s="2"/>
-    </row>
-    <row r="27" spans="1:16384">
-      <c r="A27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="9" t="str">
-        <f t="shared" ref="B27:B29" si="3">A27</f>
-        <v>&lt;!-- Twitter cards --&gt;</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD27" s="2"/>
-    </row>
-    <row r="28" spans="1:16384">
-      <c r="A28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;meta name="twitter:card" content="summary" /&gt;</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD28" s="2"/>
-    </row>
-    <row r="29" spans="1:16384">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;meta name="twitter:site" content="@ehfeduardo" /&gt;</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD29" s="2"/>
-    </row>
-    <row r="30" spans="1:16384">
-      <c r="A30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="9" t="str">
-        <f>CONCATENATE(E30,$C$1,$F$9)</f>
-        <v>&lt;meta name="twitter:title" content="Índice de Bootstrap - Ing. Eduardo Herrera Forero." /&gt;</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="XFD30" s="2"/>
-    </row>
-    <row r="31" spans="1:16384">
-      <c r="A31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="9" t="str">
-        <f>CONCATENATE(E31,$C$3,$F$9)</f>
-        <v>&lt;meta name="twitter:description" content="Este es el índice en donde se encontraran todos los artículos de la Librería CSS Bootstrap que se han publicado en este sitio web." /&gt;</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="XFD31" s="2"/>
-    </row>
-    <row r="32" spans="1:16384">
-      <c r="A32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="9" t="str">
-        <f t="shared" ref="B32:B34" si="4">A32</f>
-        <v>&lt;meta name="twitter:image" content="https://i.imgur.com/JKbKYrO.png" /&gt;</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD32" s="2"/>
-    </row>
-    <row r="33" spans="1:16384">
-      <c r="A33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;meta name="twitter:image:alt" content="Logo del ingeniero Eduardo Herrera Forero"&gt;</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD33" s="2"/>
-    </row>
-    <row r="34" spans="1:16384">
-      <c r="A34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;!-- Fin Twitter cards --&gt;</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD34" s="2"/>
-    </row>
-    <row r="35" spans="2:16384">
-      <c r="B35" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD35" s="2"/>
-    </row>
-    <row r="36" spans="1:16384">
-      <c r="A36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="9" t="str">
-        <f t="shared" ref="B36:B45" si="5">A36</f>
-        <v>&lt;!-- iconos --&gt;</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD36" s="2"/>
-    </row>
-    <row r="37" spans="1:16384">
-      <c r="A37" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;link rel="apple-touch-icon" sizes="180x180" href="apple-touch-icon.png" /&gt;</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD37" s="2"/>
-    </row>
-    <row r="38" spans="1:16384">
-      <c r="A38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;link rel="icon" type="image/png" sizes="32x32" href="favicon-32x32.png" /&gt;</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD38" s="2"/>
-    </row>
-    <row r="39" spans="1:16384">
-      <c r="A39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;link rel="icon" type="image/png" sizes="192x192" href="android-chrome-192x192.png"/&gt;</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD39" s="2"/>
-    </row>
-    <row r="40" spans="1:16384">
-      <c r="A40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;link rel="icon" type="image/png" sizes="16x16" href="favicon-16x16.png" /&gt;</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD40" s="2"/>
-    </row>
-    <row r="41" spans="1:16384">
-      <c r="A41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;link rel="manifest" href="site.webmanifest" /&gt;</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD41" s="2"/>
-    </row>
-    <row r="42" spans="1:16384">
-      <c r="A42" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;link rel="mask-icon" href="safari-pinned-tab.svg" color="#5bbad5" /&gt;</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD42" s="2"/>
-    </row>
-    <row r="43" spans="1:16384">
-      <c r="A43" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;meta name="msapplication-TileColor" content="#da532c" /&gt;</v>
-      </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD43" s="2"/>
-    </row>
-    <row r="44" spans="1:16384">
-      <c r="A44" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;meta name="theme-color" content="#ffffff" /&gt;</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD44" s="2"/>
-    </row>
-    <row r="45" spans="1:16384">
-      <c r="A45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;!-- fin iconos --&gt;</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD45" s="2"/>
-    </row>
-    <row r="46" spans="2:16384">
-      <c r="B46" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD46" s="2"/>
-    </row>
-    <row r="47" spans="1:16384">
-      <c r="A47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" s="9" t="str">
-        <f t="shared" ref="B47:B51" si="6">A47</f>
-        <v>&lt;title&gt;</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD47" s="2"/>
-    </row>
-    <row r="48" spans="1:16384">
-      <c r="A48" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="9" t="str">
-        <f>C1</f>
-        <v>Índice de Bootstrap - Ing. Eduardo Herrera Forero.</v>
-      </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD48" s="2"/>
-    </row>
-    <row r="49" spans="1:16384">
-      <c r="A49" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;/title&gt;</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD49" s="2"/>
-    </row>
-    <row r="50" spans="2:16384">
-      <c r="B50" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD50" s="2"/>
-    </row>
-    <row r="51" spans="1:16384">
-      <c r="A51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>&lt;script type="module" defer src="./js/main.js"&gt;&lt;/script&gt;</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD51" s="2"/>
-    </row>
-    <row r="52" spans="2:16384">
-      <c r="B52" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD52" s="2"/>
-    </row>
-    <row r="53" spans="1:16384">
-      <c r="A53" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="9" t="str">
-        <f>A53</f>
-        <v>&lt;meta name="google-site-verification" content="2H5ZMCD1_xl7oxaiqnopfdQBnIXVIOfmW0UBSa5sQJc"/&gt;</v>
-      </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD53" s="2"/>
-    </row>
-    <row r="54" spans="1:16384">
-      <c r="A54" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="9" t="str">
-        <f>A54</f>
-        <v>&lt;/head&gt;</v>
-      </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="XFD54" s="2"/>
-    </row>
-    <row r="55" spans="16384:16384">
-      <c r="XFD55" s="2"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/bootstrap.html"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr>
-    <tabColor theme="9" tint="0.8"/>
-  </sheetPr>
-  <dimension ref="A1:XFD54"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="0.158333333333333" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="139.991666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2"/>
-    <col min="5" max="5" width="35" style="2" customWidth="1"/>
-    <col min="6" max="16383" width="11" style="2"/>
-    <col min="16384" max="16384" width="11" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:16384">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5130,12 +4349,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add: Agregar y Quitar Objetos.html
</commit_message>
<xml_diff>
--- a/src/Head.xlsx
+++ b/src/Head.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12450" activeTab="1"/>
+    <workbookView windowWidth="27930" windowHeight="12900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="5" r:id="rId1"/>
@@ -13,11 +13,10 @@
     <sheet name="GittTABLE" sheetId="3" r:id="rId4"/>
     <sheet name="script" sheetId="8" r:id="rId5"/>
     <sheet name="plantilla" sheetId="9" r:id="rId6"/>
-    <sheet name="plantilla (2)" sheetId="10" r:id="rId7"/>
+    <sheet name="Estructura tools ps" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Comillas">plantilla!$F$1</definedName>
-    <definedName name="Comillas" localSheetId="6">'plantilla (2)'!$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="134">
   <si>
     <t>Título</t>
   </si>
@@ -225,13 +224,13 @@
     <t>&lt;/head&gt;</t>
   </si>
   <si>
-    <t>Herramientas de Selección en Photoshop - Ing. Eduardo Herrera Forero.</t>
-  </si>
-  <si>
-    <t>https://eduardoherreraf.github.io/photoshop@herramientas_de_seleccion.html</t>
-  </si>
-  <si>
-    <t>En Photoshop, las herramientas de selección son fundamentales para editar partes específicas de una imagen.</t>
+    <t>Agregar y Quitar Objetos en Photoshop - Ing. Eduardo Herrera Forero.</t>
+  </si>
+  <si>
+    <t>https://eduardoherreraf.github.io/photoshop@Agregar_y_Quitar_Objetos.html</t>
+  </si>
+  <si>
+    <t>La herramienta Parche es una herramienta poderosa en Photoshop que permite reparar y corregir áreas de una imagen de manera no destructiva. Permite al usuario seleccionar una parte de la imagen y reemplazarla con una textura o patrón tomado de otra área.</t>
   </si>
   <si>
     <t>Índice de Adobe Photoshop - Ing. Eduardo Herrera Forero.</t>
@@ -267,19 +266,78 @@
     <t>Plantilla Cuerpo</t>
   </si>
   <si>
-    <t>Plantilla Aside</t>
-  </si>
-  <si>
-    <t>&lt;main class="col-lg-8 col"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;!-- Principal  --&gt;</t>
-  </si>
-  <si>
-    <t>&lt;article class="row pb-3" id="principal"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div class="mb-n5"&gt;</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"row col"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;main class="pt-5 col-lg-9"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;article class="row border-1 border-bottom pb-3"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;</t>
   </si>
   <si>
     <t>titulo 1</t>
@@ -306,22 +364,16 @@
     <t>Agregar Objetos Mediante Clonación</t>
   </si>
   <si>
-    <t>&lt;ul class="list-unstyled px-3"&gt;</t>
-  </si>
-  <si>
     <t>&lt;div</t>
   </si>
   <si>
-    <t>&lt;li&gt;</t>
-  </si>
-  <si>
     <t>areaDeTrabajo1</t>
   </si>
   <si>
     <t>agregarObjetosMedianteClonacion</t>
   </si>
   <si>
-    <t>    class="mt-5 pt-5"&gt;</t>
+    <t>class="mt-5 pt-5"&gt;</t>
   </si>
   <si>
     <t>&lt;/div&gt;</t>
@@ -330,13 +382,13 @@
     <t>Area de trabajo 2</t>
   </si>
   <si>
-    <t>Eliminar Objetos Peqeños</t>
+    <t>Eliminar Objetos Pequeños</t>
   </si>
   <si>
     <t>areaDeTrabajo2</t>
   </si>
   <si>
-    <t>eliminarObjetosPeqeños</t>
+    <t>eliminarObjetosPequeños</t>
   </si>
   <si>
     <t>Area de trabajo 3</t>
@@ -351,10 +403,7 @@
     <t>quitarObjetos</t>
   </si>
   <si>
-    <t>class="mt-5 pt-5 mb-n5"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/ul&gt;</t>
+    <t>class="mt-5 pt-5 "&gt;</t>
   </si>
   <si>
     <t>Area de trabajo 4</t>
@@ -404,9 +453,6 @@
     </r>
   </si>
   <si>
-    <t>&lt;!-- fin Principal  --&gt;</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -436,7 +482,252 @@
     </r>
   </si>
   <si>
-    <t>Herrmientas de Selección</t>
+    <t>&lt;!-- -------------------------------- fin principal -------------------------------- --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- -------------------------------- barra lateral -------------------------------- --&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>aside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"col-lg-3 d-none d-lg-block pt-5"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Índice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;ul class="list-unstyled px-3"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>aside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;!-- -------------------------------- fin barra lateral -------------------------------- --&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Cómo usar la herramienta Parche:</t>
+  </si>
+  <si>
+    <t>1. Selecciona la herramienta Parche en la caja de herramientas de Photoshop.</t>
+  </si>
+  <si>
+    <t>2. Decide si quieres usar la opción "Parche" o "Parche de contenido":</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Parche: Toma la selección y la reemplaza por una textura tomada de otra parte de la imagen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Parche de contenido: Analiza el contenido y la textura de la selección y la reemplaza con una sección que se ajuste mejor.</t>
+  </si>
+  <si>
+    <t>3. Dibuja un área de selección alrededor de la región que quieres reparar.</t>
+  </si>
+  <si>
+    <t>4. Arrastra la selección hacia el área que quieres usar como reemplazo. Photoshop analizará la textura y el contenido y hará una sustitución coherente.</t>
+  </si>
+  <si>
+    <t>5. Ajusta la selección según sea necesario para obtener un resultado natural.</t>
+  </si>
+  <si>
+    <t>6. Repite el proceso en otras áreas que necesiten reparación.</t>
+  </si>
+  <si>
+    <t>Consejos útiles:</t>
+  </si>
+  <si>
+    <t>- Usa la herramienta Parche de contenido para reparaciones más complejas, como reemplazar caras o elementos más estructurales.</t>
+  </si>
+  <si>
+    <t>- Aumenta o disminuye el tamaño de la herramienta para ajustarse a diferentes áreas.</t>
+  </si>
+  <si>
+    <t>- Combina la herramienta Parche con otras herramientas de edición, como el clon, para obtener mejores resultados.</t>
+  </si>
+  <si>
+    <t>- Trabaja en una capa separada para mantener la edición no destructiva.</t>
   </si>
 </sst>
 </file>
@@ -450,7 +741,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +752,12 @@
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -477,9 +774,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10.5"/>
       <color rgb="FF6A9955"/>
-      <name val="Verdana"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -636,6 +939,24 @@
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -992,182 +1313,169 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="178" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2302,7 +2610,7 @@
   <dimension ref="A1:XFD55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -2422,7 +2730,7 @@
       </c>
       <c r="B9" s="23" t="str">
         <f>CONCATENATE(E9,$C$3,F9)</f>
-        <v>&lt;meta name="description" content="En Photoshop, las herramientas de selección son fundamentales para editar partes específicas de una imagen." /&gt;</v>
+        <v>&lt;meta name="description" content="La herramienta Parche es una herramienta poderosa en Photoshop que permite reparar y corregir áreas de una imagen de manera no destructiva. Permite al usuario seleccionar una parte de la imagen y reemplazarla con una textura o patrón tomado de otra área." /&gt;</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23" t="s">
@@ -2501,7 +2809,7 @@
       </c>
       <c r="B14" s="23" t="str">
         <f>CONCATENATE(E14,$C$2,$F$9)</f>
-        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/photoshop@herramientas_de_seleccion.html" /&gt;</v>
+        <v>&lt;link rel="canonical" href="https://eduardoherreraf.github.io/photoshop@Agregar_y_Quitar_Objetos.html" /&gt;</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23" t="s">
@@ -2570,7 +2878,7 @@
       </c>
       <c r="B19" s="23" t="str">
         <f>CONCATENATE(E19,$C$1,F9)</f>
-        <v>&lt;meta property="og:title" content="Herramientas de Selección en Photoshop - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta property="og:title" content="Agregar y Quitar Objetos en Photoshop - Ing. Eduardo Herrera Forero." /&gt;</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="23" t="s">
@@ -2587,7 +2895,7 @@
       </c>
       <c r="B20" s="23" t="str">
         <f>CONCATENATE(E20,$C$3,$F$9)</f>
-        <v>&lt;meta property="og:description" content="En Photoshop, las herramientas de selección son fundamentales para editar partes específicas de una imagen." /&gt;</v>
+        <v>&lt;meta property="og:description" content="La herramienta Parche es una herramienta poderosa en Photoshop que permite reparar y corregir áreas de una imagen de manera no destructiva. Permite al usuario seleccionar una parte de la imagen y reemplazarla con una textura o patrón tomado de otra área." /&gt;</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="23" t="s">
@@ -2632,7 +2940,7 @@
       </c>
       <c r="B23" s="23" t="str">
         <f>CONCATENATE(E23,$C$2,$F$9)</f>
-        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/photoshop@herramientas_de_seleccion.html" /&gt;</v>
+        <v>&lt;meta property="og:url" content="https://eduardoherreraf.github.io/photoshop@Agregar_y_Quitar_Objetos.html" /&gt;</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="23" t="s">
@@ -2729,7 +3037,7 @@
       </c>
       <c r="B30" s="23" t="str">
         <f>CONCATENATE(E30,$C$1,$F$9)</f>
-        <v>&lt;meta name="twitter:title" content="Herramientas de Selección en Photoshop - Ing. Eduardo Herrera Forero." /&gt;</v>
+        <v>&lt;meta name="twitter:title" content="Agregar y Quitar Objetos en Photoshop - Ing. Eduardo Herrera Forero." /&gt;</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="23" t="s">
@@ -2746,7 +3054,7 @@
       </c>
       <c r="B31" s="23" t="str">
         <f>CONCATENATE(E31,$C$3,$F$9)</f>
-        <v>&lt;meta name="twitter:description" content="En Photoshop, las herramientas de selección son fundamentales para editar partes específicas de una imagen." /&gt;</v>
+        <v>&lt;meta name="twitter:description" content="La herramienta Parche es una herramienta poderosa en Photoshop que permite reparar y corregir áreas de una imagen de manera no destructiva. Permite al usuario seleccionar una parte de la imagen y reemplazarla con una textura o patrón tomado de otra área." /&gt;</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="23" t="s">
@@ -2979,7 +3287,7 @@
       </c>
       <c r="B48" s="23" t="str">
         <f>C1</f>
-        <v>Herramientas de Selección en Photoshop - Ing. Eduardo Herrera Forero.</v>
+        <v>Agregar y Quitar Objetos en Photoshop - Ing. Eduardo Herrera Forero.</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="23" t="s">
@@ -3068,7 +3376,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/photoshop@herramientas_de_seleccion.html" tooltip="https://eduardoherreraf.github.io/photoshop@herramientas_de_seleccion.html"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://eduardoherreraf.github.io/photoshop@Agregar_y_Quitar_Objetos.html" tooltip="https://eduardoherreraf.github.io/photoshop@Agregar_y_Quitar_Objetos.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4656,10 +4964,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -4668,8 +4976,8 @@
     <col min="2" max="2" width="0.158333333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="50.75" style="3" customWidth="1"/>
     <col min="4" max="4" width="0.158333333333333" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="0.325" style="2" customWidth="1"/>
+    <col min="5" max="5" width="104.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="0.158333333333333" style="2" customWidth="1"/>
     <col min="7" max="7" width="94.625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
@@ -4688,23 +4996,23 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="3:7">
+    <row r="3" spans="3:5">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="4" spans="3:4">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="3:4">
+    <row r="5" spans="3:5">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
+      <c r="E5" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="3:5">
       <c r="C6" s="2"/>
@@ -4716,22 +5024,23 @@
     <row r="7" spans="3:5">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="4" t="s">
-        <v>78</v>
+      <c r="E7" s="4" t="str">
+        <f>CONCATENATE("&lt;!--  ",$C$11,"  --&gt;")</f>
+        <v>&lt;!--  Agregar y quitar objetos  --&gt;</v>
       </c>
     </row>
     <row r="8" spans="3:5">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="3:5">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="3:5">
@@ -4744,52 +5053,52 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" spans="1:6">
+      <c r="A12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:6">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="D12" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="7" t="str">
+        <v>82</v>
+      </c>
+      <c r="E12" s="4" t="str">
         <f>IF(C12&lt;&gt;"",C12,"")</f>
         <v>Agregar y quitar objetos en Photoshop se refiere al proceso de modificar una imagen digital añadiendo nuevos elementos o eliminando elementos existentes. Es una técnica esencial en el diseño gráfico, la fotografía y el diseño web.</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="28" t="s">
-        <v>83</v>
+      <c r="C13" s="7"/>
+      <c r="D13" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="E13" s="4" t="str">
         <f>IF(C13&lt;&gt;"",C13,"")</f>
@@ -4810,73 +5119,59 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="4" t="str">
         <f>CONCATENATE("&lt;!-- ",C15," --&gt;")</f>
         <v>&lt;!-- Agregar Objetos Mediante Clonación --&gt;</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
+    </row>
+    <row r="16" spans="2:5">
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="4" t="str">
         <f>CONCATENATE("id=",Comillas,C17,Comillas)</f>
         <v>id="agregarObjetosMedianteClonacion"</v>
       </c>
-      <c r="G17" s="9" t="str">
-        <f>CONCATENATE("&lt;a href=",Comillas,"#",C17,Comillas,"&gt;",C15,"&lt;/a&gt;")</f>
-        <v>&lt;a href="#agregarObjetosMedianteClonacion"&gt;Agregar Objetos Mediante Clonación&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="9" t="str">
-        <f>IF($C$15&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="19" ht="30" spans="2:7">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
@@ -4886,11 +5181,6 @@
         <f>CONCATENATE("&lt;h2 class=",Comillas,"mt-1",Comillas,"&gt;",C15,"&lt;/h2&gt;")</f>
         <v>&lt;h2 class="mt-1"&gt;Agregar Objetos Mediante Clonación&lt;/h2&gt;</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9" t="str">
-        <f>IF(C$21&lt;&gt;"","&lt;li&gt;","")</f>
-        <v>&lt;li&gt;</v>
-      </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="2" t="s">
@@ -4898,32 +5188,30 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="9" t="str">
-        <f>IF(C$21&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C23,Comillas,"&gt;",C21,"&lt;/a&gt;"),"")</f>
-        <v>&lt;a href="#eliminarObjetosPeqeños"&gt;Eliminar Objetos Peqeños&lt;/a&gt;</v>
+      <c r="E20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="8"/>
+      <c r="C21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="4" t="str">
         <f>IF(C21&lt;&gt;"",CONCATENATE("&lt;!-- ",C21," --&gt;"),"")</f>
-        <v>&lt;!-- Eliminar Objetos Peqeños --&gt;</v>
-      </c>
-      <c r="G21" s="9" t="str">
-        <f>IF($C$21&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
+        <v>&lt;!-- Eliminar Objetos Pequeños --&gt;</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -4932,33 +5220,31 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="10" t="str">
+      <c r="E22" s="8" t="str">
         <f>IF(C21&lt;&gt;"","&lt;div","")</f>
         <v>&lt;div</v>
       </c>
-      <c r="G22" s="9" t="str">
-        <f>IF($C$27&lt;&gt;"","&lt;li&gt;","")</f>
-        <v>&lt;li&gt;</v>
+      <c r="G22" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="8"/>
+      <c r="C23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="4" t="str">
         <f>IF(C21&lt;&gt;"",CONCATENATE("id=",Comillas,C23,Comillas),"")</f>
-        <v>id="eliminarObjetosPeqeños"</v>
-      </c>
-      <c r="G23" s="9" t="str">
-        <f>IF($C$27&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C29,Comillas,"&gt;",C27,"&lt;/a&gt;"),"")</f>
-        <v>&lt;a href="#quitarObjetos"&gt;Quitar Objetos&lt;/a&gt;</v>
+        <v>id="eliminarObjetosPequeños"</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:7">
@@ -4969,14 +5255,13 @@
       <c r="D24" s="2"/>
       <c r="E24" s="4" t="str">
         <f>IF(C21&lt;&gt;"",F29,"")</f>
-        <v>class="mt-5 pt-5 mb-n5"&gt;</v>
-      </c>
-      <c r="G24" s="9" t="str">
-        <f>IF($C$27&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="25" ht="30" spans="2:7">
+        <v>class="mt-5 pt-5 "&gt;</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
@@ -4984,11 +5269,10 @@
       <c r="D25" s="2"/>
       <c r="E25" s="4" t="str">
         <f>IF(C21&lt;&gt;"",CONCATENATE("&lt;h2 class=",Comillas,"mt-1",Comillas,"&gt;",C21,"&lt;/h2&gt;"),"")</f>
-        <v>&lt;h2 class="mt-1"&gt;Eliminar Objetos Peqeños&lt;/h2&gt;</v>
-      </c>
-      <c r="G25" s="9" t="str">
-        <f>IF($C$33&lt;&gt;"","&lt;li&gt;","")</f>
-        <v>&lt;li&gt;</v>
+        <v>&lt;h2 class="mt-1"&gt;Eliminar Objetos Pequeños&lt;/h2&gt;</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:7">
@@ -4997,33 +5281,31 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="10" t="str">
+      <c r="E26" s="8" t="str">
         <f>IF(C21&lt;&gt;"","&lt;/div&gt;","")</f>
         <v>&lt;/div&gt;</v>
       </c>
-      <c r="G26" s="9" t="str">
-        <f>IF($C$33&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C35,Comillas,"&gt;",C33,"&lt;/a&gt;"),"")</f>
-        <v>&lt;a href="#MejorasOpcionesSeleccion"&gt;Herramienta Parche (Patch Tool)&lt;/a&gt;</v>
+      <c r="G26" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="8"/>
+      <c r="C27" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="7"/>
       <c r="E27" s="4" t="str">
         <f>IF(C27&lt;&gt;"",CONCATENATE("&lt;!-- ",C27," --&gt;"),"")</f>
         <v>&lt;!-- Quitar Objetos --&gt;</v>
       </c>
-      <c r="G27" s="9" t="str">
-        <f>IF($C$33&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
+      <c r="G27" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:7">
@@ -5032,36 +5314,34 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="10" t="str">
+      <c r="E28" s="8" t="str">
         <f>IF(C27&lt;&gt;"","&lt;div","")</f>
         <v>&lt;div</v>
       </c>
-      <c r="G28" s="9" t="str">
-        <f>IF($C$39&lt;&gt;"","&lt;li&gt;","")</f>
-        <v/>
+      <c r="G28" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="8"/>
+      <c r="C29" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="7"/>
       <c r="E29" s="4" t="str">
         <f>IF(C27&lt;&gt;"",CONCATENATE("id=",Comillas,C29,Comillas),"")</f>
         <v>id="quitarObjetos"</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="9" t="str">
-        <f>IF($C$39&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C41,Comillas,"&gt;",C39,"&lt;/a&gt;"),"")</f>
-        <v/>
+      <c r="F29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:7">
@@ -5072,11 +5352,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="4" t="str">
         <f>IF(C27&lt;&gt;"",F35,"")</f>
-        <v>class="mt-5 pt-5 mb-n5"&gt;</v>
-      </c>
-      <c r="G30" s="9" t="str">
-        <f>IF($C$39&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v/>
+        <v>class="mt-5 pt-5 "&gt;</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:7">
@@ -5089,36 +5368,42 @@
         <f>IF(C27&lt;&gt;"",CONCATENATE("&lt;h2 class=",Comillas,"mt-1",Comillas,"&gt;",C27,"&lt;/h2&gt;"),"")</f>
         <v>&lt;h2 class="mt-1"&gt;Quitar Objetos&lt;/h2&gt;</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
+      <c r="G31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="10" t="str">
+      <c r="E32" s="8" t="str">
         <f>IF(C27&lt;&gt;"","&lt;/div&gt;","")</f>
         <v>&lt;/div&gt;</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7" t="str">
+      <c r="C33" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="4" t="str">
         <f>IF(C33&lt;&gt;"",CONCATENATE("&lt;!-- ",C33," --&gt;"),"")</f>
         <v>&lt;!-- Herramienta Parche (Patch Tool) --&gt;</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="2" t="s">
@@ -5126,7 +5411,7 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="10" t="str">
+      <c r="E34" s="8" t="str">
         <f>IF(C33&lt;&gt;"","&lt;div","")</f>
         <v>&lt;div</v>
       </c>
@@ -5136,27 +5421,27 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="8"/>
+      <c r="C35" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="7"/>
       <c r="E35" s="4" t="str">
         <f>IF(C33&lt;&gt;"",CONCATENATE("id=",Comillas,C35,Comillas),"")</f>
         <v>id="MejorasOpcionesSeleccion"</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>104</v>
+      <c r="F35" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:7">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -5164,77 +5449,101 @@
       <c r="D36" s="2"/>
       <c r="E36" s="4" t="str">
         <f>IF(C33&lt;&gt;"",F41,"")</f>
-        <v>class="mt-5 pt-5 mb-n5"&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
+        <v>class="mt-5 pt-5 "&gt;</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="7" t="str">
+      <c r="E37" s="4" t="str">
         <f>IF(C33&lt;&gt;"",CONCATENATE("&lt;h2 class=",Comillas,"mt-1",Comillas,"&gt;",C33,"&lt;/h2&gt;"),"")</f>
         <v>&lt;h2 class="mt-1"&gt;Herramienta Parche (Patch Tool)&lt;/h2&gt;</v>
       </c>
-    </row>
-    <row r="38" spans="2:5">
+      <c r="F37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
       <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="10" t="str">
+      <c r="E38" s="8" t="str">
         <f>IF(C33&lt;&gt;"","&lt;/div&gt;","")</f>
         <v>&lt;/div&gt;</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="G38" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
       <c r="E39" s="4" t="str">
         <f>IF(C39&lt;&gt;"",CONCATENATE("&lt;!-- ",C39," --&gt;"),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="2:5">
+      <c r="F39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
       <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="10" t="str">
+      <c r="E40" s="8" t="str">
         <f>IF(C39&lt;&gt;"","&lt;div","")</f>
         <v/>
       </c>
+      <c r="F40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
       <c r="E41" s="4" t="str">
         <f>IF(C39&lt;&gt;"",CONCATENATE("id=",Comillas,C41,Comillas),"")</f>
         <v/>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>104</v>
+      <c r="F41" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:7">
       <c r="B42" s="2" t="s">
         <v>2</v>
       </c>
@@ -5242,8 +5551,11 @@
         <f>IF(C39&lt;&gt;"",F48,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="2:5">
+      <c r="G42" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
       <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
@@ -5251,107 +5563,252 @@
         <f>IF(C39&lt;&gt;"",CONCATENATE("&lt;h2 class=",Comillas,"mt-1",Comillas,"&gt;",C39,"&lt;/h2&gt;"),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="2:5">
+      <c r="G43" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
       <c r="B44" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="10" t="str">
+      <c r="E44" s="8" t="str">
         <f>IF(C39&lt;&gt;"","&lt;/div&gt;","")</f>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="2:5">
+      <c r="G44" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
       <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5">
+      <c r="E45" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
       <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <f>CONCATENATE("&lt;!--  ",$C$11,"  --&gt;")</f>
+        <v>&lt;!--  Agregar y quitar objetos  --&gt;</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="G50" s="13"/>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E47" s="13" t="s">
+    <row r="52" spans="2:5">
+      <c r="B52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="2:7">
-      <c r="B48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E48" s="14" t="s">
+      <c r="F53" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
+      <c r="F54" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
       <c r="B55" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="2:2">
+      <c r="E55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
       <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="2:2">
+      <c r="E56" s="2" t="str">
+        <f>CONCATENATE("&lt;a href=",Comillas,"#",C17,Comillas,"&gt;",C15,"&lt;/a&gt;")</f>
+        <v>&lt;a href="#agregarObjetosMedianteClonacion"&gt;Agregar Objetos Mediante Clonación&lt;/a&gt;</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
       <c r="B57" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="2:2">
+      <c r="E57" s="2" t="str">
+        <f>IF($C$15&lt;&gt;"","&lt;/li&gt;","")</f>
+        <v>&lt;/li&gt;</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
       <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="2:2">
+      <c r="E58" s="2" t="str">
+        <f>IF(C$21&lt;&gt;"","&lt;li&gt;","")</f>
+        <v>&lt;li&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
       <c r="B59" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="E59" s="2" t="str">
+        <f>IF(C$21&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C23,Comillas,"&gt;",C21,"&lt;/a&gt;"),"")</f>
+        <v>&lt;a href="#eliminarObjetosPequeños"&gt;Eliminar Objetos Pequeños&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5">
+      <c r="E60" s="2" t="str">
+        <f>IF($C$21&lt;&gt;"","&lt;/li&gt;","")</f>
+        <v>&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5">
+      <c r="E61" s="2" t="str">
+        <f>IF($C$27&lt;&gt;"","&lt;li&gt;","")</f>
+        <v>&lt;li&gt;</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5">
+      <c r="E62" s="2" t="str">
+        <f>IF($C$27&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C29,Comillas,"&gt;",C27,"&lt;/a&gt;"),"")</f>
+        <v>&lt;a href="#quitarObjetos"&gt;Quitar Objetos&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5">
+      <c r="E63" s="2" t="str">
+        <f>IF($C$27&lt;&gt;"","&lt;/li&gt;","")</f>
+        <v>&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="64" spans="5:5">
+      <c r="E64" s="2" t="str">
+        <f>IF($C$33&lt;&gt;"","&lt;li&gt;","")</f>
+        <v>&lt;li&gt;</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5">
+      <c r="E65" s="2" t="str">
+        <f>IF($C$33&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C35,Comillas,"&gt;",C33,"&lt;/a&gt;"),"")</f>
+        <v>&lt;a href="#MejorasOpcionesSeleccion"&gt;Herramienta Parche (Patch Tool)&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5">
+      <c r="E66" s="2" t="str">
+        <f>IF($C$33&lt;&gt;"","&lt;/li&gt;","")</f>
+        <v>&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5">
+      <c r="E67" s="2" t="str">
+        <f>IF($C$39&lt;&gt;"","&lt;li&gt;","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="5:5">
+      <c r="E68" s="2" t="str">
+        <f>IF($C$39&lt;&gt;"",CONCATENATE("&lt;a href=",Comillas,"#",C41,Comillas,"&gt;",C39,"&lt;/a&gt;"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="5:5">
+      <c r="E69" s="2" t="str">
+        <f>IF($C$39&lt;&gt;"","&lt;/li&gt;","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="5:5">
+      <c r="E70" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5">
+      <c r="E71" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5">
+      <c r="E72" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5">
+      <c r="E73" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -5369,711 +5826,93 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="0.158333333333333" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.75" style="3" customWidth="1"/>
-    <col min="4" max="4" width="0.158333333333333" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="0.325" style="2" customWidth="1"/>
-    <col min="7" max="7" width="94.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="2"/>
+    <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6">
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="3:4">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="3:7">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="3:4">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="3:5">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4" t="str">
-        <f>CONCATENATE("&lt;h1&gt;",C11,"&lt;/h1&gt;")</f>
-        <v>&lt;h1&gt;Herrmientas de Selección&lt;/h1&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="7" t="str">
-        <f>IF(C12&lt;&gt;"",C12,"")</f>
-        <v>Agregar y quitar objetos en Photoshop se refiere al proceso de modificar una imagen digital añadiendo nuevos elementos o eliminando elementos existentes. Es una técnica esencial en el diseño gráfico, la fotografía y el diseño web.</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="4" t="str">
-        <f>IF(C13&lt;&gt;"",C13,"")</f>
-        <v/>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4" t="str">
-        <f>IF(C13&lt;&gt;"",CONCATENATE("&lt;p&gt;",C13,"&lt;/p&gt;"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="4" t="str">
-        <f>CONCATENATE("&lt;!-- ",C15," --&gt;")</f>
-        <v>&lt;!-- Agregar Objetos Mediante Clonación --&gt;</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="4" t="str">
-        <f>CONCATENATE("id=",'plantilla (2)'!Comillas,C17,'plantilla (2)'!Comillas)</f>
-        <v>id="agregarObjetosMedianteClonacion"</v>
-      </c>
-      <c r="G17" s="9" t="str">
-        <f>CONCATENATE("&lt;a href=",'plantilla (2)'!Comillas,"#",C17,'plantilla (2)'!Comillas,"&gt;",C15,"&lt;/a&gt;")</f>
-        <v>&lt;a href="#agregarObjetosMedianteClonacion"&gt;Agregar Objetos Mediante Clonación&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="9" t="str">
-        <f>IF($C$15&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="19" ht="30" spans="2:7">
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4" t="str">
-        <f>CONCATENATE("&lt;h2 class=",'plantilla (2)'!Comillas,"mt-1",'plantilla (2)'!Comillas,"&gt;",C15,"&lt;/h2&gt;")</f>
-        <v>&lt;h2 class="mt-1"&gt;Agregar Objetos Mediante Clonación&lt;/h2&gt;</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9" t="str">
-        <f>IF(C$21&lt;&gt;"","&lt;li&gt;","")</f>
-        <v>&lt;li&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="9" t="str">
-        <f>IF(C$21&lt;&gt;"",CONCATENATE("&lt;a href=",'plantilla (2)'!Comillas,"#",C23,'plantilla (2)'!Comillas,"&gt;",C21,"&lt;/a&gt;"),"")</f>
-        <v>&lt;a href="#eliminarObjetosPeqeños"&gt;Eliminar Objetos Peqeños&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="4" t="str">
-        <f>IF(C21&lt;&gt;"",CONCATENATE("&lt;!-- ",C21," --&gt;"),"")</f>
-        <v>&lt;!-- Eliminar Objetos Peqeños --&gt;</v>
-      </c>
-      <c r="G21" s="9" t="str">
-        <f>IF($C$21&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="10" t="str">
-        <f>IF(C21&lt;&gt;"","&lt;div","")</f>
-        <v>&lt;div</v>
-      </c>
-      <c r="G22" s="9" t="str">
-        <f>IF($C$27&lt;&gt;"","&lt;li&gt;","")</f>
-        <v>&lt;li&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="4" t="str">
-        <f>IF(C21&lt;&gt;"",CONCATENATE("id=",'plantilla (2)'!Comillas,C23,'plantilla (2)'!Comillas),"")</f>
-        <v>id="eliminarObjetosPeqeños"</v>
-      </c>
-      <c r="G23" s="9" t="str">
-        <f>IF($C$27&lt;&gt;"",CONCATENATE("&lt;a href=",'plantilla (2)'!Comillas,"#",C29,'plantilla (2)'!Comillas,"&gt;",C27,"&lt;/a&gt;"),"")</f>
-        <v>&lt;a href="#quitarObjetos"&gt;Quitar Objetos&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4" t="str">
-        <f>IF(C21&lt;&gt;"",F29,"")</f>
-        <v>class="mt-5 pt-5 mb-n5"&gt;</v>
-      </c>
-      <c r="G24" s="9" t="str">
-        <f>IF($C$27&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="25" ht="30" spans="2:7">
-      <c r="B25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="4" t="str">
-        <f>IF(C21&lt;&gt;"",CONCATENATE("&lt;h2 class=",'plantilla (2)'!Comillas,"mt-1",'plantilla (2)'!Comillas,"&gt;",C21,"&lt;/h2&gt;"),"")</f>
-        <v>&lt;h2 class="mt-1"&gt;Eliminar Objetos Peqeños&lt;/h2&gt;</v>
-      </c>
-      <c r="G25" s="9" t="str">
-        <f>IF($C$33&lt;&gt;"","&lt;li&gt;","")</f>
-        <v>&lt;li&gt;</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="10" t="str">
-        <f>IF(C21&lt;&gt;"","&lt;/div&gt;","")</f>
-        <v>&lt;/div&gt;</v>
-      </c>
-      <c r="G26" s="9" t="str">
-        <f>IF($C$33&lt;&gt;"",CONCATENATE("&lt;a href=",'plantilla (2)'!Comillas,"#",C35,'plantilla (2)'!Comillas,"&gt;",C33,"&lt;/a&gt;"),"")</f>
-        <v>&lt;a href="#MejorasOpcionesSeleccion"&gt;Herramienta Parche (Patch Tool)&lt;/a&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="4" t="str">
-        <f>IF(C27&lt;&gt;"",CONCATENATE("&lt;!-- ",C27," --&gt;"),"")</f>
-        <v>&lt;!-- Quitar Objetos --&gt;</v>
-      </c>
-      <c r="G27" s="9" t="str">
-        <f>IF($C$33&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v>&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="10" t="str">
-        <f>IF(C27&lt;&gt;"","&lt;div","")</f>
-        <v>&lt;div</v>
-      </c>
-      <c r="G28" s="9" t="str">
-        <f>IF($C$39&lt;&gt;"","&lt;li&gt;","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="4" t="str">
-        <f>IF(C27&lt;&gt;"",CONCATENATE("id=",'plantilla (2)'!Comillas,C29,'plantilla (2)'!Comillas),"")</f>
-        <v>id="quitarObjetos"</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="9" t="str">
-        <f>IF($C$39&lt;&gt;"",CONCATENATE("&lt;a href=",'plantilla (2)'!Comillas,"#",C41,'plantilla (2)'!Comillas,"&gt;",C39,"&lt;/a&gt;"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="4" t="str">
-        <f>IF(C27&lt;&gt;"",F35,"")</f>
-        <v>class="mt-5 pt-5 mb-n5"&gt;</v>
-      </c>
-      <c r="G30" s="9" t="str">
-        <f>IF($C$39&lt;&gt;"","&lt;/li&gt;","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="4" t="str">
-        <f>IF(C27&lt;&gt;"",CONCATENATE("&lt;h2 class=",'plantilla (2)'!Comillas,"mt-1",'plantilla (2)'!Comillas,"&gt;",C27,"&lt;/h2&gt;"),"")</f>
-        <v>&lt;h2 class="mt-1"&gt;Quitar Objetos&lt;/h2&gt;</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="10" t="str">
-        <f>IF(C27&lt;&gt;"","&lt;/div&gt;","")</f>
-        <v>&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7" t="str">
-        <f>IF(C33&lt;&gt;"",CONCATENATE("&lt;!-- ",C33," --&gt;"),"")</f>
-        <v>&lt;!-- Herramienta Parche (Patch Tool) --&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="10" t="str">
-        <f>IF(C33&lt;&gt;"","&lt;div","")</f>
-        <v>&lt;div</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="4" t="str">
-        <f>IF(C33&lt;&gt;"",CONCATENATE("id=",'plantilla (2)'!Comillas,C35,'plantilla (2)'!Comillas),"")</f>
-        <v>id="MejorasOpcionesSeleccion"</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="4" t="str">
-        <f>IF(C33&lt;&gt;"",F41,"")</f>
-        <v>class="mt-5 pt-5 mb-n5"&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="7" t="str">
-        <f>IF(C33&lt;&gt;"",CONCATENATE("&lt;h2 class=",'plantilla (2)'!Comillas,"mt-1",'plantilla (2)'!Comillas,"&gt;",C33,"&lt;/h2&gt;"),"")</f>
-        <v>&lt;h2 class="mt-1"&gt;Herramienta Parche (Patch Tool)&lt;/h2&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="10" t="str">
-        <f>IF(C33&lt;&gt;"","&lt;/div&gt;","")</f>
-        <v>&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="4" t="str">
-        <f>IF(C39&lt;&gt;"",CONCATENATE("&lt;!-- ",C39," --&gt;"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="10" t="str">
-        <f>IF(C39&lt;&gt;"","&lt;div","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="4" t="str">
-        <f>IF(C39&lt;&gt;"",CONCATENATE("id=",'plantilla (2)'!Comillas,C41,'plantilla (2)'!Comillas),"")</f>
-        <v/>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="4" t="str">
-        <f>IF(C39&lt;&gt;"",F48,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="4" t="str">
-        <f>IF(C39&lt;&gt;"",CONCATENATE("&lt;h2 class=",'plantilla (2)'!Comillas,"mt-1",'plantilla (2)'!Comillas,"&gt;",C39,"&lt;/h2&gt;"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="10" t="str">
-        <f>IF(C39&lt;&gt;"","&lt;/div&gt;","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7">
-      <c r="B48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="2" t="s">
-        <v>2</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C$1:D$1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" location="HerramientaMarcoRectangular" display="Agregar Objetos Mediante Clonación"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>